<commit_message>
Linux Chrome Driver added and Code Updated
</commit_message>
<xml_diff>
--- a/Datasources/JSDProjectdata.xlsx
+++ b/Datasources/JSDProjectdata.xlsx
@@ -116,7 +116,7 @@
     <t>harsha</t>
   </si>
   <si>
-    <t>Rakesh1234$</t>
+    <t>Rakesh123$</t>
   </si>
 </sst>
 </file>
@@ -719,7 +719,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>

</xml_diff>